<commit_message>
just for recording: Implementing authentication issues.
</commit_message>
<xml_diff>
--- a/meta/samples/pages/ChartSample.xlsx
+++ b/meta/samples/pages/ChartSample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yhaino/Desktop/dapanda-front-core/meta/samples/pages/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/dapanda/dapanda-front-core/meta/samples/pages/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99189A85-109D-974C-B050-CD5A7B2FF313}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{647CB30D-0594-4445-86B3-0A83B612E8F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3600" yWindow="500" windowWidth="25200" windowHeight="17500" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="112">
   <si>
     <t>パッケージ</t>
   </si>
@@ -934,6 +934,52 @@
   </si>
   <si>
     <t>{color: "red"}</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>BeforeRouteLeave関数名</t>
+    <rPh sb="16" eb="18">
+      <t xml:space="preserve">カンスウ </t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t xml:space="preserve">メイ </t>
+    </rPh>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>RouterHooks.beforeRouteLeave</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>/* BeforeRouteLeave関数を実装する場合はここに関数名を定義し、Vueコンポーネント定義・ヘッダ情報（コンポーネント定義用）に関数のインポートを定義します。 */</t>
+    <rPh sb="19" eb="21">
+      <t xml:space="preserve">カンスウ </t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t xml:space="preserve">ジッソウ </t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t xml:space="preserve">バアイハ </t>
+    </rPh>
+    <rPh sb="32" eb="35">
+      <t xml:space="preserve">カンスウメイヲ </t>
+    </rPh>
+    <rPh sb="36" eb="38">
+      <t xml:space="preserve">テイギシ </t>
+    </rPh>
+    <rPh sb="47" eb="50">
+      <t xml:space="preserve">テイギヨウ </t>
+    </rPh>
+    <rPh sb="71" eb="73">
+      <t xml:space="preserve">カンスウ </t>
+    </rPh>
+    <rPh sb="80" eb="82">
+      <t xml:space="preserve">テイギ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>import { RouterHooks } from "@/utils/RouterHooks"</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -1746,53 +1792,53 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2205,10 +2251,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M97"/>
+  <dimension ref="A1:M98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="E67" sqref="E67"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -2323,10 +2369,10 @@
       <c r="I9" s="35"/>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="103" t="s">
+      <c r="A10" s="102" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="104"/>
+      <c r="B10" s="103"/>
       <c r="C10" s="10" t="s">
         <v>90</v>
       </c>
@@ -2340,10 +2386,10 @@
       <c r="I10" s="35"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="103" t="s">
+      <c r="A11" s="102" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="104"/>
+      <c r="B11" s="103"/>
       <c r="C11" s="10" t="s">
         <v>91</v>
       </c>
@@ -2357,10 +2403,10 @@
       <c r="I11" s="35"/>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="103" t="s">
+      <c r="A12" s="102" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="104"/>
+      <c r="B12" s="103"/>
       <c r="C12" s="10" t="s">
         <v>21</v>
       </c>
@@ -2374,10 +2420,10 @@
       <c r="I12" s="35"/>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="103" t="s">
+      <c r="A13" s="102" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="104"/>
+      <c r="B13" s="103"/>
       <c r="C13" s="86" t="s">
         <v>48</v>
       </c>
@@ -2395,11 +2441,11 @@
         <v>1</v>
       </c>
       <c r="B14" s="6"/>
-      <c r="C14" s="105" t="s">
+      <c r="C14" s="104" t="s">
         <v>89</v>
       </c>
-      <c r="D14" s="106"/>
-      <c r="E14" s="107"/>
+      <c r="D14" s="105"/>
+      <c r="E14" s="106"/>
       <c r="F14" s="65"/>
       <c r="G14" s="65"/>
       <c r="H14" s="65"/>
@@ -2540,10 +2586,10 @@
       <c r="I22"/>
     </row>
     <row r="23" spans="1:13" s="32" customFormat="1">
-      <c r="A23" s="95" t="s">
+      <c r="A23" s="107" t="s">
         <v>60</v>
       </c>
-      <c r="B23" s="96"/>
+      <c r="B23" s="108"/>
       <c r="C23" s="64"/>
       <c r="D23" t="s">
         <v>58</v>
@@ -2555,31 +2601,31 @@
       <c r="I23"/>
     </row>
     <row r="24" spans="1:13" s="32" customFormat="1">
-      <c r="A24" s="62" t="s">
-        <v>15</v>
-      </c>
-      <c r="B24" s="63"/>
+      <c r="A24" s="107" t="s">
+        <v>108</v>
+      </c>
+      <c r="B24" s="108"/>
       <c r="C24" s="64" t="s">
-        <v>14</v>
-      </c>
-      <c r="D24"/>
+        <v>109</v>
+      </c>
+      <c r="D24" t="s">
+        <v>110</v>
+      </c>
       <c r="E24"/>
       <c r="F24"/>
-      <c r="G24" s="66"/>
-      <c r="H24" s="66"/>
+      <c r="G24"/>
+      <c r="H24"/>
       <c r="I24"/>
     </row>
     <row r="25" spans="1:13" s="32" customFormat="1">
-      <c r="A25" s="95" t="s">
-        <v>18</v>
-      </c>
-      <c r="B25" s="96"/>
+      <c r="A25" s="62" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" s="63"/>
       <c r="C25" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="D25" t="s">
-        <v>19</v>
-      </c>
+      <c r="D25"/>
       <c r="E25"/>
       <c r="F25"/>
       <c r="G25" s="66"/>
@@ -2587,96 +2633,98 @@
       <c r="I25"/>
     </row>
     <row r="26" spans="1:13" s="32" customFormat="1">
-      <c r="A26" s="95" t="s">
-        <v>49</v>
-      </c>
-      <c r="B26" s="96"/>
+      <c r="A26" s="107" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="108"/>
       <c r="C26" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="D26"/>
+      <c r="D26" t="s">
+        <v>19</v>
+      </c>
       <c r="E26"/>
       <c r="F26"/>
       <c r="G26" s="66"/>
       <c r="H26" s="66"/>
       <c r="I26"/>
     </row>
-    <row r="27" spans="1:13" s="37" customFormat="1">
-      <c r="A27" s="34"/>
-      <c r="B27" s="36"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="34"/>
-      <c r="I27" s="34"/>
-      <c r="J27" s="34"/>
-      <c r="K27" s="34"/>
-    </row>
-    <row r="28" spans="1:13">
-      <c r="A28" s="30" t="s">
+    <row r="27" spans="1:13" s="32" customFormat="1">
+      <c r="A27" s="107" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="108"/>
+      <c r="C27" s="64" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27"/>
+      <c r="E27"/>
+      <c r="F27"/>
+      <c r="G27" s="66"/>
+      <c r="H27" s="66"/>
+      <c r="I27"/>
+    </row>
+    <row r="28" spans="1:13" s="37" customFormat="1">
+      <c r="A28" s="34"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="34"/>
+      <c r="D28" s="34"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="34"/>
+      <c r="G28" s="34"/>
+      <c r="H28" s="34"/>
+      <c r="I28" s="34"/>
+      <c r="J28" s="34"/>
+      <c r="K28" s="34"/>
+    </row>
+    <row r="29" spans="1:13">
+      <c r="A29" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="B28" s="31"/>
-      <c r="C28" s="31"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="81"/>
-      <c r="F28" s="44" t="s">
+      <c r="B29" s="31"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="81"/>
+      <c r="F29" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="G28" s="44"/>
-      <c r="H28" s="44"/>
-      <c r="I28" s="44"/>
-      <c r="J28" s="43"/>
-      <c r="K28" s="43"/>
-      <c r="L28" s="43"/>
-      <c r="M28" s="43"/>
-    </row>
-    <row r="29" spans="1:13">
-      <c r="A29" s="47" t="s">
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="43"/>
+      <c r="K29" s="43"/>
+      <c r="L29" s="43"/>
+      <c r="M29" s="43"/>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="A30" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B29" s="42" t="s">
+      <c r="B30" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="42"/>
-      <c r="D29" s="42"/>
-      <c r="E29" s="82"/>
-      <c r="F29" s="67"/>
-      <c r="G29" s="67"/>
-      <c r="H29" s="67"/>
-      <c r="I29" s="67"/>
-      <c r="J29" s="44"/>
-      <c r="K29" s="45"/>
-      <c r="L29" s="45"/>
-      <c r="M29" s="35"/>
-    </row>
-    <row r="30" spans="1:13">
-      <c r="A30" s="51">
+      <c r="C30" s="42"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="82"/>
+      <c r="F30" s="67"/>
+      <c r="G30" s="67"/>
+      <c r="H30" s="67"/>
+      <c r="I30" s="67"/>
+      <c r="J30" s="44"/>
+      <c r="K30" s="45"/>
+      <c r="L30" s="45"/>
+      <c r="M30" s="35"/>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="A31" s="51">
         <v>1</v>
       </c>
-      <c r="B30" s="46" t="s">
+      <c r="B31" s="46" t="s">
         <v>102</v>
       </c>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="39"/>
-      <c r="F30" s="68"/>
-      <c r="G30" s="68"/>
-      <c r="H30" s="68"/>
-      <c r="I30" s="34"/>
-      <c r="J30" s="36"/>
-      <c r="K30" s="36"/>
-      <c r="L30" s="36"/>
-      <c r="M30" s="35"/>
-    </row>
-    <row r="31" spans="1:13">
-      <c r="A31" s="51"/>
-      <c r="B31" s="46"/>
-      <c r="C31" s="40"/>
-      <c r="D31" s="40"/>
-      <c r="E31" s="41"/>
+      <c r="C31" s="38"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="39"/>
       <c r="F31" s="68"/>
       <c r="G31" s="68"/>
       <c r="H31" s="68"/>
@@ -2687,11 +2735,15 @@
       <c r="M31" s="35"/>
     </row>
     <row r="32" spans="1:13">
-      <c r="A32" s="52"/>
-      <c r="B32" s="48"/>
-      <c r="C32" s="49"/>
-      <c r="D32" s="49"/>
-      <c r="E32" s="50"/>
+      <c r="A32" s="51">
+        <v>2</v>
+      </c>
+      <c r="B32" s="46" t="s">
+        <v>111</v>
+      </c>
+      <c r="C32" s="40"/>
+      <c r="D32" s="40"/>
+      <c r="E32" s="41"/>
       <c r="F32" s="68"/>
       <c r="G32" s="68"/>
       <c r="H32" s="68"/>
@@ -2702,80 +2754,80 @@
       <c r="M32" s="35"/>
     </row>
     <row r="33" spans="1:13">
-      <c r="A33" s="13"/>
-      <c r="B33" s="13"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
-      <c r="H33" s="13"/>
-      <c r="I33" s="13"/>
-      <c r="J33" s="13"/>
+      <c r="A33" s="52"/>
+      <c r="B33" s="48"/>
+      <c r="C33" s="49"/>
+      <c r="D33" s="49"/>
+      <c r="E33" s="50"/>
+      <c r="F33" s="68"/>
+      <c r="G33" s="68"/>
+      <c r="H33" s="68"/>
+      <c r="I33" s="34"/>
+      <c r="J33" s="36"/>
+      <c r="K33" s="36"/>
+      <c r="L33" s="36"/>
+      <c r="M33" s="35"/>
     </row>
     <row r="34" spans="1:13">
-      <c r="A34" s="30" t="s">
+      <c r="A34" s="13"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="13"/>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="B34" s="31"/>
-      <c r="C34" s="31"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="81"/>
-      <c r="F34" s="44" t="s">
+      <c r="B35" s="31"/>
+      <c r="C35" s="31"/>
+      <c r="D35" s="31"/>
+      <c r="E35" s="81"/>
+      <c r="F35" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="G34" s="44"/>
-      <c r="H34" s="44"/>
-      <c r="I34" s="44"/>
-      <c r="J34" s="43"/>
-      <c r="K34" s="43"/>
-      <c r="L34" s="43"/>
-      <c r="M34" s="43"/>
-    </row>
-    <row r="35" spans="1:13">
-      <c r="A35" s="47" t="s">
+      <c r="G35" s="44"/>
+      <c r="H35" s="44"/>
+      <c r="I35" s="44"/>
+      <c r="J35" s="43"/>
+      <c r="K35" s="43"/>
+      <c r="L35" s="43"/>
+      <c r="M35" s="43"/>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B35" s="42" t="s">
+      <c r="B36" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="C35" s="42"/>
-      <c r="D35" s="42"/>
-      <c r="E35" s="82"/>
-      <c r="F35" s="67"/>
-      <c r="G35" s="67"/>
-      <c r="H35" s="67"/>
-      <c r="I35" s="67"/>
-      <c r="J35" s="44"/>
-      <c r="K35" s="45"/>
-      <c r="L35" s="45"/>
-      <c r="M35" s="35"/>
-    </row>
-    <row r="36" spans="1:13">
-      <c r="A36" s="51">
+      <c r="C36" s="42"/>
+      <c r="D36" s="42"/>
+      <c r="E36" s="82"/>
+      <c r="F36" s="67"/>
+      <c r="G36" s="67"/>
+      <c r="H36" s="67"/>
+      <c r="I36" s="67"/>
+      <c r="J36" s="44"/>
+      <c r="K36" s="45"/>
+      <c r="L36" s="45"/>
+      <c r="M36" s="35"/>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37" s="51">
         <v>1</v>
       </c>
-      <c r="B36" s="46" t="s">
+      <c r="B37" s="46" t="s">
         <v>101</v>
       </c>
-      <c r="C36" s="38"/>
-      <c r="D36" s="38"/>
-      <c r="E36" s="39"/>
-      <c r="F36" s="68"/>
-      <c r="G36" s="68"/>
-      <c r="H36" s="68"/>
-      <c r="I36" s="34"/>
-      <c r="J36" s="36"/>
-      <c r="K36" s="36"/>
-      <c r="L36" s="36"/>
-      <c r="M36" s="35"/>
-    </row>
-    <row r="37" spans="1:13">
-      <c r="A37" s="51"/>
-      <c r="B37" s="46"/>
-      <c r="C37" s="40"/>
-      <c r="D37" s="40"/>
-      <c r="E37" s="41"/>
+      <c r="C37" s="38"/>
+      <c r="D37" s="38"/>
+      <c r="E37" s="39"/>
       <c r="F37" s="68"/>
       <c r="G37" s="68"/>
       <c r="H37" s="68"/>
@@ -2786,11 +2838,11 @@
       <c r="M37" s="35"/>
     </row>
     <row r="38" spans="1:13">
-      <c r="A38" s="52"/>
-      <c r="B38" s="48"/>
-      <c r="C38" s="49"/>
-      <c r="D38" s="49"/>
-      <c r="E38" s="50"/>
+      <c r="A38" s="51"/>
+      <c r="B38" s="46"/>
+      <c r="C38" s="40"/>
+      <c r="D38" s="40"/>
+      <c r="E38" s="41"/>
       <c r="F38" s="68"/>
       <c r="G38" s="68"/>
       <c r="H38" s="68"/>
@@ -2801,11 +2853,11 @@
       <c r="M38" s="35"/>
     </row>
     <row r="39" spans="1:13">
-      <c r="A39" s="83"/>
-      <c r="B39" s="84"/>
-      <c r="C39" s="85"/>
-      <c r="D39" s="85"/>
-      <c r="E39" s="85"/>
+      <c r="A39" s="52"/>
+      <c r="B39" s="48"/>
+      <c r="C39" s="49"/>
+      <c r="D39" s="49"/>
+      <c r="E39" s="50"/>
       <c r="F39" s="68"/>
       <c r="G39" s="68"/>
       <c r="H39" s="68"/>
@@ -2816,64 +2868,64 @@
       <c r="M39" s="35"/>
     </row>
     <row r="40" spans="1:13">
-      <c r="A40" s="30" t="s">
+      <c r="A40" s="83"/>
+      <c r="B40" s="84"/>
+      <c r="C40" s="85"/>
+      <c r="D40" s="85"/>
+      <c r="E40" s="85"/>
+      <c r="F40" s="68"/>
+      <c r="G40" s="68"/>
+      <c r="H40" s="68"/>
+      <c r="I40" s="34"/>
+      <c r="J40" s="36"/>
+      <c r="K40" s="36"/>
+      <c r="L40" s="36"/>
+      <c r="M40" s="35"/>
+    </row>
+    <row r="41" spans="1:13">
+      <c r="A41" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="B40" s="31"/>
-      <c r="C40" s="31"/>
-      <c r="D40" s="31"/>
-      <c r="E40" s="81"/>
-      <c r="F40" s="44" t="s">
+      <c r="B41" s="31"/>
+      <c r="C41" s="31"/>
+      <c r="D41" s="31"/>
+      <c r="E41" s="81"/>
+      <c r="F41" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="G40" s="44"/>
-      <c r="H40" s="44"/>
-      <c r="I40" s="44"/>
-      <c r="J40" s="43"/>
-      <c r="K40" s="43"/>
-      <c r="L40" s="43"/>
-      <c r="M40" s="43"/>
-    </row>
-    <row r="41" spans="1:13">
-      <c r="A41" s="47" t="s">
+      <c r="G41" s="44"/>
+      <c r="H41" s="44"/>
+      <c r="I41" s="44"/>
+      <c r="J41" s="43"/>
+      <c r="K41" s="43"/>
+      <c r="L41" s="43"/>
+      <c r="M41" s="43"/>
+    </row>
+    <row r="42" spans="1:13">
+      <c r="A42" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B41" s="42" t="s">
+      <c r="B42" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="C41" s="42"/>
-      <c r="D41" s="42"/>
-      <c r="E41" s="82"/>
-      <c r="F41" s="67"/>
-      <c r="G41" s="67"/>
-      <c r="H41" s="67"/>
-      <c r="I41" s="67"/>
-      <c r="J41" s="44"/>
-      <c r="K41" s="45"/>
-      <c r="L41" s="45"/>
-      <c r="M41" s="35"/>
-    </row>
-    <row r="42" spans="1:13">
-      <c r="A42" s="51"/>
-      <c r="B42" s="46"/>
-      <c r="C42" s="38"/>
-      <c r="D42" s="38"/>
-      <c r="E42" s="39"/>
-      <c r="F42" s="68"/>
-      <c r="G42" s="68"/>
-      <c r="H42" s="68"/>
-      <c r="I42" s="34"/>
-      <c r="J42" s="36"/>
-      <c r="K42" s="36"/>
-      <c r="L42" s="36"/>
+      <c r="C42" s="42"/>
+      <c r="D42" s="42"/>
+      <c r="E42" s="82"/>
+      <c r="F42" s="67"/>
+      <c r="G42" s="67"/>
+      <c r="H42" s="67"/>
+      <c r="I42" s="67"/>
+      <c r="J42" s="44"/>
+      <c r="K42" s="45"/>
+      <c r="L42" s="45"/>
       <c r="M42" s="35"/>
     </row>
     <row r="43" spans="1:13">
       <c r="A43" s="51"/>
       <c r="B43" s="46"/>
-      <c r="C43" s="40"/>
-      <c r="D43" s="40"/>
-      <c r="E43" s="41"/>
+      <c r="C43" s="38"/>
+      <c r="D43" s="38"/>
+      <c r="E43" s="39"/>
       <c r="F43" s="68"/>
       <c r="G43" s="68"/>
       <c r="H43" s="68"/>
@@ -2884,11 +2936,11 @@
       <c r="M43" s="35"/>
     </row>
     <row r="44" spans="1:13">
-      <c r="A44" s="52"/>
-      <c r="B44" s="48"/>
-      <c r="C44" s="49"/>
-      <c r="D44" s="49"/>
-      <c r="E44" s="50"/>
+      <c r="A44" s="51"/>
+      <c r="B44" s="46"/>
+      <c r="C44" s="40"/>
+      <c r="D44" s="40"/>
+      <c r="E44" s="41"/>
       <c r="F44" s="68"/>
       <c r="G44" s="68"/>
       <c r="H44" s="68"/>
@@ -2899,80 +2951,80 @@
       <c r="M44" s="35"/>
     </row>
     <row r="45" spans="1:13">
-      <c r="A45" s="13"/>
-      <c r="B45" s="13"/>
-      <c r="C45" s="13"/>
-      <c r="D45" s="13"/>
-      <c r="E45" s="13"/>
-      <c r="F45" s="13"/>
-      <c r="G45" s="13"/>
-      <c r="H45" s="13"/>
-      <c r="I45" s="13"/>
-      <c r="J45" s="13"/>
+      <c r="A45" s="52"/>
+      <c r="B45" s="48"/>
+      <c r="C45" s="49"/>
+      <c r="D45" s="49"/>
+      <c r="E45" s="50"/>
+      <c r="F45" s="68"/>
+      <c r="G45" s="68"/>
+      <c r="H45" s="68"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="36"/>
+      <c r="K45" s="36"/>
+      <c r="L45" s="36"/>
+      <c r="M45" s="35"/>
     </row>
     <row r="46" spans="1:13">
-      <c r="A46" s="30" t="s">
+      <c r="A46" s="13"/>
+      <c r="B46" s="13"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="13"/>
+      <c r="I46" s="13"/>
+      <c r="J46" s="13"/>
+    </row>
+    <row r="47" spans="1:13">
+      <c r="A47" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="B46" s="31"/>
-      <c r="C46" s="31"/>
-      <c r="D46" s="31"/>
-      <c r="E46" s="81"/>
-      <c r="F46" s="44" t="s">
+      <c r="B47" s="31"/>
+      <c r="C47" s="31"/>
+      <c r="D47" s="31"/>
+      <c r="E47" s="81"/>
+      <c r="F47" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="G46" s="44"/>
-      <c r="H46" s="44"/>
-      <c r="I46" s="44"/>
-      <c r="J46" s="43"/>
-      <c r="K46" s="43"/>
-      <c r="L46" s="43"/>
-      <c r="M46" s="43"/>
-    </row>
-    <row r="47" spans="1:13">
-      <c r="A47" s="47" t="s">
+      <c r="G47" s="44"/>
+      <c r="H47" s="44"/>
+      <c r="I47" s="44"/>
+      <c r="J47" s="43"/>
+      <c r="K47" s="43"/>
+      <c r="L47" s="43"/>
+      <c r="M47" s="43"/>
+    </row>
+    <row r="48" spans="1:13">
+      <c r="A48" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B47" s="42" t="s">
+      <c r="B48" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="C47" s="47" t="s">
+      <c r="C48" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="D47" s="42" t="s">
+      <c r="D48" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="E47" s="82"/>
-      <c r="F47" s="67"/>
-      <c r="G47" s="67"/>
-      <c r="H47" s="67"/>
-      <c r="I47" s="67"/>
-      <c r="J47" s="44"/>
-      <c r="K47" s="45"/>
-      <c r="L47" s="45"/>
-      <c r="M47" s="35"/>
-    </row>
-    <row r="48" spans="1:13">
-      <c r="A48" s="51"/>
-      <c r="B48" s="46"/>
-      <c r="C48" s="87"/>
-      <c r="D48" s="38"/>
-      <c r="E48" s="39"/>
-      <c r="F48" s="68"/>
-      <c r="G48" s="68"/>
-      <c r="H48" s="68"/>
-      <c r="I48" s="34"/>
-      <c r="J48" s="36"/>
-      <c r="K48" s="36"/>
-      <c r="L48" s="36"/>
+      <c r="E48" s="82"/>
+      <c r="F48" s="67"/>
+      <c r="G48" s="67"/>
+      <c r="H48" s="67"/>
+      <c r="I48" s="67"/>
+      <c r="J48" s="44"/>
+      <c r="K48" s="45"/>
+      <c r="L48" s="45"/>
       <c r="M48" s="35"/>
     </row>
     <row r="49" spans="1:13">
       <c r="A49" s="51"/>
       <c r="B49" s="46"/>
-      <c r="C49" s="88"/>
-      <c r="D49" s="40"/>
-      <c r="E49" s="41"/>
+      <c r="C49" s="87"/>
+      <c r="D49" s="38"/>
+      <c r="E49" s="39"/>
       <c r="F49" s="68"/>
       <c r="G49" s="68"/>
       <c r="H49" s="68"/>
@@ -2983,11 +3035,11 @@
       <c r="M49" s="35"/>
     </row>
     <row r="50" spans="1:13">
-      <c r="A50" s="52"/>
-      <c r="B50" s="48"/>
-      <c r="C50" s="89"/>
-      <c r="D50" s="49"/>
-      <c r="E50" s="50"/>
+      <c r="A50" s="51"/>
+      <c r="B50" s="46"/>
+      <c r="C50" s="88"/>
+      <c r="D50" s="40"/>
+      <c r="E50" s="41"/>
       <c r="F50" s="68"/>
       <c r="G50" s="68"/>
       <c r="H50" s="68"/>
@@ -2998,11 +3050,11 @@
       <c r="M50" s="35"/>
     </row>
     <row r="51" spans="1:13">
-      <c r="A51" s="83"/>
-      <c r="B51" s="84"/>
-      <c r="C51" s="85"/>
-      <c r="D51" s="85"/>
-      <c r="E51" s="85"/>
+      <c r="A51" s="52"/>
+      <c r="B51" s="48"/>
+      <c r="C51" s="89"/>
+      <c r="D51" s="49"/>
+      <c r="E51" s="50"/>
       <c r="F51" s="68"/>
       <c r="G51" s="68"/>
       <c r="H51" s="68"/>
@@ -3013,66 +3065,66 @@
       <c r="M51" s="35"/>
     </row>
     <row r="52" spans="1:13">
-      <c r="A52" s="30" t="s">
+      <c r="A52" s="83"/>
+      <c r="B52" s="84"/>
+      <c r="C52" s="85"/>
+      <c r="D52" s="85"/>
+      <c r="E52" s="85"/>
+      <c r="F52" s="68"/>
+      <c r="G52" s="68"/>
+      <c r="H52" s="68"/>
+      <c r="I52" s="34"/>
+      <c r="J52" s="36"/>
+      <c r="K52" s="36"/>
+      <c r="L52" s="36"/>
+      <c r="M52" s="35"/>
+    </row>
+    <row r="53" spans="1:13">
+      <c r="A53" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="B52" s="31"/>
-      <c r="C52" s="31"/>
-      <c r="D52" s="31"/>
-      <c r="E52" s="81"/>
-      <c r="F52" s="44" t="s">
+      <c r="B53" s="31"/>
+      <c r="C53" s="31"/>
+      <c r="D53" s="31"/>
+      <c r="E53" s="81"/>
+      <c r="F53" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="G52" s="44"/>
-      <c r="H52" s="44"/>
-      <c r="I52" s="44"/>
-      <c r="J52" s="43"/>
-      <c r="K52" s="43"/>
-      <c r="L52" s="43"/>
-      <c r="M52" s="43"/>
-    </row>
-    <row r="53" spans="1:13">
-      <c r="A53" s="47" t="s">
+      <c r="G53" s="44"/>
+      <c r="H53" s="44"/>
+      <c r="I53" s="44"/>
+      <c r="J53" s="43"/>
+      <c r="K53" s="43"/>
+      <c r="L53" s="43"/>
+      <c r="M53" s="43"/>
+    </row>
+    <row r="54" spans="1:13">
+      <c r="A54" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B53" s="42" t="s">
+      <c r="B54" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="C53" s="42"/>
-      <c r="D53" s="42"/>
-      <c r="E53" s="82"/>
-      <c r="F53" s="67" t="s">
+      <c r="C54" s="42"/>
+      <c r="D54" s="42"/>
+      <c r="E54" s="82"/>
+      <c r="F54" s="67" t="s">
         <v>80</v>
       </c>
-      <c r="G53" s="67"/>
-      <c r="H53" s="67"/>
-      <c r="I53" s="67"/>
-      <c r="J53" s="44"/>
-      <c r="K53" s="45"/>
-      <c r="L53" s="45"/>
-      <c r="M53" s="35"/>
-    </row>
-    <row r="54" spans="1:13">
-      <c r="A54" s="51"/>
-      <c r="B54" s="46"/>
-      <c r="C54" s="38"/>
-      <c r="D54" s="38"/>
-      <c r="E54" s="39"/>
-      <c r="F54" s="68"/>
-      <c r="G54" s="68"/>
-      <c r="H54" s="68"/>
-      <c r="I54" s="34"/>
-      <c r="J54" s="36"/>
-      <c r="K54" s="36"/>
-      <c r="L54" s="36"/>
+      <c r="G54" s="67"/>
+      <c r="H54" s="67"/>
+      <c r="I54" s="67"/>
+      <c r="J54" s="44"/>
+      <c r="K54" s="45"/>
+      <c r="L54" s="45"/>
       <c r="M54" s="35"/>
     </row>
     <row r="55" spans="1:13">
       <c r="A55" s="51"/>
       <c r="B55" s="46"/>
-      <c r="C55" s="40"/>
-      <c r="D55" s="40"/>
-      <c r="E55" s="41"/>
+      <c r="C55" s="38"/>
+      <c r="D55" s="38"/>
+      <c r="E55" s="39"/>
       <c r="F55" s="68"/>
       <c r="G55" s="68"/>
       <c r="H55" s="68"/>
@@ -3083,11 +3135,11 @@
       <c r="M55" s="35"/>
     </row>
     <row r="56" spans="1:13">
-      <c r="A56" s="52"/>
-      <c r="B56" s="48"/>
-      <c r="C56" s="49"/>
-      <c r="D56" s="49"/>
-      <c r="E56" s="50"/>
+      <c r="A56" s="51"/>
+      <c r="B56" s="46"/>
+      <c r="C56" s="40"/>
+      <c r="D56" s="40"/>
+      <c r="E56" s="41"/>
       <c r="F56" s="68"/>
       <c r="G56" s="68"/>
       <c r="H56" s="68"/>
@@ -3098,22 +3150,23 @@
       <c r="M56" s="35"/>
     </row>
     <row r="57" spans="1:13">
-      <c r="A57" s="13"/>
-      <c r="B57" s="13"/>
-      <c r="C57" s="13"/>
-      <c r="D57" s="13"/>
-      <c r="E57" s="13"/>
-      <c r="F57" s="13"/>
-      <c r="G57" s="13"/>
-      <c r="H57" s="13"/>
-      <c r="I57" s="13"/>
-      <c r="J57" s="13"/>
+      <c r="A57" s="52"/>
+      <c r="B57" s="48"/>
+      <c r="C57" s="49"/>
+      <c r="D57" s="49"/>
+      <c r="E57" s="50"/>
+      <c r="F57" s="68"/>
+      <c r="G57" s="68"/>
+      <c r="H57" s="68"/>
+      <c r="I57" s="34"/>
+      <c r="J57" s="36"/>
+      <c r="K57" s="36"/>
+      <c r="L57" s="36"/>
+      <c r="M57" s="35"/>
     </row>
     <row r="58" spans="1:13">
       <c r="A58" s="13"/>
-      <c r="B58" s="13" t="s">
-        <v>61</v>
-      </c>
+      <c r="B58" s="13"/>
       <c r="C58" s="13"/>
       <c r="D58" s="13"/>
       <c r="E58" s="13"/>
@@ -3124,115 +3177,103 @@
       <c r="J58" s="13"/>
     </row>
     <row r="59" spans="1:13">
-      <c r="A59" s="3" t="s">
+      <c r="A59" s="13"/>
+      <c r="B59" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C59" s="13"/>
+      <c r="D59" s="13"/>
+      <c r="E59" s="13"/>
+      <c r="F59" s="13"/>
+      <c r="G59" s="13"/>
+      <c r="H59" s="13"/>
+      <c r="I59" s="13"/>
+      <c r="J59" s="13"/>
+    </row>
+    <row r="60" spans="1:13">
+      <c r="A60" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B59" s="14"/>
-      <c r="C59" s="14"/>
-      <c r="D59" s="14"/>
-      <c r="E59" s="14"/>
-      <c r="F59" s="14"/>
-      <c r="G59" s="14"/>
-      <c r="H59" s="14"/>
-      <c r="I59" s="14"/>
-      <c r="J59" s="14"/>
-      <c r="K59" s="14"/>
-      <c r="L59" s="6"/>
-      <c r="M59" s="15"/>
-    </row>
-    <row r="60" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A60" s="98" t="s">
+      <c r="B60" s="14"/>
+      <c r="C60" s="14"/>
+      <c r="D60" s="14"/>
+      <c r="E60" s="14"/>
+      <c r="F60" s="14"/>
+      <c r="G60" s="14"/>
+      <c r="H60" s="14"/>
+      <c r="I60" s="14"/>
+      <c r="J60" s="14"/>
+      <c r="K60" s="14"/>
+      <c r="L60" s="6"/>
+      <c r="M60" s="15"/>
+    </row>
+    <row r="61" spans="1:13" ht="13.5" customHeight="1">
+      <c r="A61" s="101" t="s">
         <v>7</v>
       </c>
-      <c r="B60" s="98" t="s">
+      <c r="B61" s="101" t="s">
         <v>3</v>
       </c>
-      <c r="C60" s="97" t="s">
+      <c r="C61" s="98" t="s">
         <v>4</v>
       </c>
-      <c r="D60" s="97" t="s">
+      <c r="D61" s="98" t="s">
         <v>6</v>
       </c>
-      <c r="E60" s="97" t="s">
+      <c r="E61" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="F60" s="101" t="s">
+      <c r="F61" s="99" t="s">
         <v>33</v>
       </c>
-      <c r="G60" s="101" t="s">
+      <c r="G61" s="99" t="s">
         <v>16</v>
       </c>
-      <c r="H60" s="99" t="s">
+      <c r="H61" s="109" t="s">
         <v>81</v>
       </c>
-      <c r="I60" s="97" t="s">
+      <c r="I61" s="98" t="s">
         <v>1</v>
       </c>
-      <c r="J60" s="97"/>
-      <c r="K60" s="16"/>
-      <c r="L60" s="17"/>
-      <c r="M60" s="9"/>
-    </row>
-    <row r="61" spans="1:13">
-      <c r="A61" s="98"/>
-      <c r="B61" s="98"/>
-      <c r="C61" s="97"/>
-      <c r="D61" s="97"/>
-      <c r="E61" s="97"/>
-      <c r="F61" s="102"/>
-      <c r="G61" s="102"/>
-      <c r="H61" s="100"/>
-      <c r="I61" s="97"/>
-      <c r="J61" s="97"/>
-      <c r="K61" s="18"/>
-      <c r="L61" s="29"/>
-      <c r="M61" s="15"/>
+      <c r="J61" s="98"/>
+      <c r="K61" s="16"/>
+      <c r="L61" s="17"/>
+      <c r="M61" s="9"/>
     </row>
     <row r="62" spans="1:13">
-      <c r="A62" s="19">
-        <v>1</v>
-      </c>
-      <c r="B62" s="71" t="s">
-        <v>92</v>
-      </c>
-      <c r="C62" s="78" t="s">
-        <v>93</v>
-      </c>
-      <c r="D62" s="20"/>
-      <c r="E62" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="F62" s="20"/>
-      <c r="G62" s="69"/>
-      <c r="H62" s="69"/>
-      <c r="I62" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="J62" s="21"/>
-      <c r="K62" s="21"/>
-      <c r="L62" s="28"/>
+      <c r="A62" s="101"/>
+      <c r="B62" s="101"/>
+      <c r="C62" s="98"/>
+      <c r="D62" s="98"/>
+      <c r="E62" s="98"/>
+      <c r="F62" s="100"/>
+      <c r="G62" s="100"/>
+      <c r="H62" s="110"/>
+      <c r="I62" s="98"/>
+      <c r="J62" s="98"/>
+      <c r="K62" s="18"/>
+      <c r="L62" s="29"/>
       <c r="M62" s="15"/>
     </row>
     <row r="63" spans="1:13">
       <c r="A63" s="19">
-        <f>A62+1</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B63" s="71" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C63" s="78" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D63" s="20"/>
-      <c r="E63" s="20">
-        <v>400</v>
+      <c r="E63" s="20" t="s">
+        <v>103</v>
       </c>
       <c r="F63" s="20"/>
       <c r="G63" s="69"/>
       <c r="H63" s="69"/>
       <c r="I63" s="20" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="J63" s="21"/>
       <c r="K63" s="21"/>
@@ -3241,13 +3282,13 @@
     </row>
     <row r="64" spans="1:13">
       <c r="A64" s="19">
-        <f t="shared" ref="A64:A78" si="0">A63+1</f>
-        <v>3</v>
-      </c>
-      <c r="B64" s="72" t="s">
-        <v>95</v>
-      </c>
-      <c r="C64" s="79" t="s">
+        <f>A63+1</f>
+        <v>2</v>
+      </c>
+      <c r="B64" s="71" t="s">
+        <v>94</v>
+      </c>
+      <c r="C64" s="78" t="s">
         <v>97</v>
       </c>
       <c r="D64" s="20"/>
@@ -3258,32 +3299,34 @@
       <c r="G64" s="69"/>
       <c r="H64" s="69"/>
       <c r="I64" s="20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J64" s="21"/>
       <c r="K64" s="21"/>
-      <c r="L64" s="22"/>
+      <c r="L64" s="28"/>
       <c r="M64" s="15"/>
     </row>
     <row r="65" spans="1:13">
       <c r="A65" s="19">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B65" s="73" t="s">
-        <v>96</v>
-      </c>
-      <c r="C65" s="80" t="s">
-        <v>93</v>
+        <f t="shared" ref="A65:A79" si="0">A64+1</f>
+        <v>3</v>
+      </c>
+      <c r="B65" s="72" t="s">
+        <v>95</v>
+      </c>
+      <c r="C65" s="79" t="s">
+        <v>97</v>
       </c>
       <c r="D65" s="20"/>
-      <c r="E65" s="94" t="s">
-        <v>104</v>
+      <c r="E65" s="20">
+        <v>400</v>
       </c>
       <c r="F65" s="20"/>
       <c r="G65" s="69"/>
       <c r="H65" s="69"/>
-      <c r="I65" s="20"/>
+      <c r="I65" s="20" t="s">
+        <v>99</v>
+      </c>
       <c r="J65" s="21"/>
       <c r="K65" s="21"/>
       <c r="L65" s="22"/>
@@ -3292,17 +3335,17 @@
     <row r="66" spans="1:13">
       <c r="A66" s="19">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B66" s="73" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="C66" s="80" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="D66" s="20"/>
-      <c r="E66" s="20" t="s">
-        <v>107</v>
+      <c r="E66" s="94" t="s">
+        <v>104</v>
       </c>
       <c r="F66" s="20"/>
       <c r="G66" s="69"/>
@@ -3316,61 +3359,67 @@
     <row r="67" spans="1:13">
       <c r="A67" s="19">
         <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B67" s="73"/>
-      <c r="C67" s="80"/>
-      <c r="D67" s="74"/>
-      <c r="E67" s="74"/>
-      <c r="F67" s="74"/>
-      <c r="G67" s="75"/>
-      <c r="H67" s="75"/>
-      <c r="I67" s="74"/>
-      <c r="J67" s="76"/>
-      <c r="K67" s="76"/>
-      <c r="L67" s="77"/>
+        <v>5</v>
+      </c>
+      <c r="B67" s="73" t="s">
+        <v>105</v>
+      </c>
+      <c r="C67" s="80" t="s">
+        <v>106</v>
+      </c>
+      <c r="D67" s="20"/>
+      <c r="E67" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="F67" s="20"/>
+      <c r="G67" s="69"/>
+      <c r="H67" s="69"/>
+      <c r="I67" s="20"/>
+      <c r="J67" s="21"/>
+      <c r="K67" s="21"/>
+      <c r="L67" s="22"/>
       <c r="M67" s="15"/>
     </row>
     <row r="68" spans="1:13">
       <c r="A68" s="19">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B68" s="73"/>
       <c r="C68" s="80"/>
-      <c r="D68" s="20"/>
-      <c r="E68" s="20"/>
-      <c r="F68" s="20"/>
-      <c r="G68" s="69"/>
-      <c r="H68" s="69"/>
-      <c r="I68" s="20"/>
-      <c r="J68" s="21"/>
-      <c r="K68" s="21"/>
-      <c r="L68" s="22"/>
+      <c r="D68" s="74"/>
+      <c r="E68" s="74"/>
+      <c r="F68" s="74"/>
+      <c r="G68" s="75"/>
+      <c r="H68" s="75"/>
+      <c r="I68" s="74"/>
+      <c r="J68" s="76"/>
+      <c r="K68" s="76"/>
+      <c r="L68" s="77"/>
       <c r="M68" s="15"/>
     </row>
     <row r="69" spans="1:13">
       <c r="A69" s="19">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B69" s="73"/>
       <c r="C69" s="80"/>
-      <c r="D69" s="74"/>
-      <c r="E69" s="74"/>
-      <c r="F69" s="74"/>
-      <c r="G69" s="75"/>
-      <c r="H69" s="75"/>
-      <c r="I69" s="74"/>
-      <c r="J69" s="76"/>
-      <c r="K69" s="76"/>
-      <c r="L69" s="77"/>
+      <c r="D69" s="20"/>
+      <c r="E69" s="20"/>
+      <c r="F69" s="20"/>
+      <c r="G69" s="69"/>
+      <c r="H69" s="69"/>
+      <c r="I69" s="20"/>
+      <c r="J69" s="21"/>
+      <c r="K69" s="21"/>
+      <c r="L69" s="22"/>
       <c r="M69" s="15"/>
     </row>
     <row r="70" spans="1:13">
       <c r="A70" s="19">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B70" s="73"/>
       <c r="C70" s="80"/>
@@ -3388,43 +3437,43 @@
     <row r="71" spans="1:13">
       <c r="A71" s="19">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B71" s="73"/>
       <c r="C71" s="80"/>
-      <c r="D71" s="20"/>
-      <c r="E71" s="20"/>
-      <c r="F71" s="20"/>
-      <c r="G71" s="69"/>
-      <c r="H71" s="69"/>
-      <c r="I71" s="20"/>
-      <c r="J71" s="21"/>
-      <c r="K71" s="21"/>
-      <c r="L71" s="22"/>
+      <c r="D71" s="74"/>
+      <c r="E71" s="74"/>
+      <c r="F71" s="74"/>
+      <c r="G71" s="75"/>
+      <c r="H71" s="75"/>
+      <c r="I71" s="74"/>
+      <c r="J71" s="76"/>
+      <c r="K71" s="76"/>
+      <c r="L71" s="77"/>
       <c r="M71" s="15"/>
     </row>
     <row r="72" spans="1:13">
       <c r="A72" s="19">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B72" s="73"/>
       <c r="C72" s="80"/>
-      <c r="D72" s="74"/>
-      <c r="E72" s="74"/>
-      <c r="F72" s="74"/>
-      <c r="G72" s="75"/>
-      <c r="H72" s="75"/>
-      <c r="I72" s="74"/>
-      <c r="J72" s="76"/>
-      <c r="K72" s="76"/>
-      <c r="L72" s="77"/>
+      <c r="D72" s="20"/>
+      <c r="E72" s="20"/>
+      <c r="F72" s="20"/>
+      <c r="G72" s="69"/>
+      <c r="H72" s="69"/>
+      <c r="I72" s="20"/>
+      <c r="J72" s="21"/>
+      <c r="K72" s="21"/>
+      <c r="L72" s="22"/>
       <c r="M72" s="15"/>
     </row>
     <row r="73" spans="1:13">
       <c r="A73" s="19">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B73" s="73"/>
       <c r="C73" s="80"/>
@@ -3442,43 +3491,43 @@
     <row r="74" spans="1:13">
       <c r="A74" s="19">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B74" s="73"/>
       <c r="C74" s="80"/>
-      <c r="D74" s="20"/>
-      <c r="E74" s="20"/>
-      <c r="F74" s="20"/>
-      <c r="G74" s="69"/>
-      <c r="H74" s="69"/>
-      <c r="I74" s="20"/>
-      <c r="J74" s="21"/>
-      <c r="K74" s="21"/>
-      <c r="L74" s="22"/>
+      <c r="D74" s="74"/>
+      <c r="E74" s="74"/>
+      <c r="F74" s="74"/>
+      <c r="G74" s="75"/>
+      <c r="H74" s="75"/>
+      <c r="I74" s="74"/>
+      <c r="J74" s="76"/>
+      <c r="K74" s="76"/>
+      <c r="L74" s="77"/>
       <c r="M74" s="15"/>
     </row>
     <row r="75" spans="1:13">
       <c r="A75" s="19">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B75" s="73"/>
       <c r="C75" s="80"/>
-      <c r="D75" s="74"/>
-      <c r="E75" s="74"/>
-      <c r="F75" s="74"/>
-      <c r="G75" s="75"/>
-      <c r="H75" s="75"/>
-      <c r="I75" s="74"/>
-      <c r="J75" s="76"/>
-      <c r="K75" s="76"/>
-      <c r="L75" s="77"/>
+      <c r="D75" s="20"/>
+      <c r="E75" s="20"/>
+      <c r="F75" s="20"/>
+      <c r="G75" s="69"/>
+      <c r="H75" s="69"/>
+      <c r="I75" s="20"/>
+      <c r="J75" s="21"/>
+      <c r="K75" s="21"/>
+      <c r="L75" s="22"/>
       <c r="M75" s="15"/>
     </row>
     <row r="76" spans="1:13">
       <c r="A76" s="19">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B76" s="73"/>
       <c r="C76" s="80"/>
@@ -3496,113 +3545,116 @@
     <row r="77" spans="1:13">
       <c r="A77" s="19">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B77" s="73"/>
       <c r="C77" s="80"/>
-      <c r="D77" s="20"/>
-      <c r="E77" s="20"/>
-      <c r="F77" s="20"/>
-      <c r="G77" s="69"/>
-      <c r="H77" s="69"/>
-      <c r="I77" s="20"/>
-      <c r="J77" s="21"/>
-      <c r="K77" s="21"/>
-      <c r="L77" s="22"/>
+      <c r="D77" s="74"/>
+      <c r="E77" s="74"/>
+      <c r="F77" s="74"/>
+      <c r="G77" s="75"/>
+      <c r="H77" s="75"/>
+      <c r="I77" s="74"/>
+      <c r="J77" s="76"/>
+      <c r="K77" s="76"/>
+      <c r="L77" s="77"/>
       <c r="M77" s="15"/>
     </row>
     <row r="78" spans="1:13">
       <c r="A78" s="19">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B78" s="73"/>
       <c r="C78" s="80"/>
-      <c r="D78" s="74"/>
-      <c r="E78" s="74"/>
-      <c r="F78" s="74"/>
-      <c r="G78" s="75"/>
-      <c r="H78" s="75"/>
-      <c r="I78" s="74"/>
-      <c r="J78" s="76"/>
-      <c r="K78" s="76"/>
-      <c r="L78" s="77"/>
+      <c r="D78" s="20"/>
+      <c r="E78" s="20"/>
+      <c r="F78" s="20"/>
+      <c r="G78" s="69"/>
+      <c r="H78" s="69"/>
+      <c r="I78" s="20"/>
+      <c r="J78" s="21"/>
+      <c r="K78" s="21"/>
+      <c r="L78" s="22"/>
       <c r="M78" s="15"/>
     </row>
     <row r="79" spans="1:13">
-      <c r="A79" s="23"/>
-      <c r="B79" s="24"/>
-      <c r="C79" s="25"/>
-      <c r="D79" s="25"/>
-      <c r="E79" s="25"/>
-      <c r="F79" s="25"/>
-      <c r="G79" s="70"/>
-      <c r="H79" s="70"/>
-      <c r="I79" s="25"/>
-      <c r="J79" s="26"/>
-      <c r="K79" s="26"/>
-      <c r="L79" s="27"/>
+      <c r="A79" s="19">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B79" s="73"/>
+      <c r="C79" s="80"/>
+      <c r="D79" s="74"/>
+      <c r="E79" s="74"/>
+      <c r="F79" s="74"/>
+      <c r="G79" s="75"/>
+      <c r="H79" s="75"/>
+      <c r="I79" s="74"/>
+      <c r="J79" s="76"/>
+      <c r="K79" s="76"/>
+      <c r="L79" s="77"/>
       <c r="M79" s="15"/>
     </row>
-    <row r="81" spans="1:13">
-      <c r="A81" s="30" t="s">
+    <row r="80" spans="1:13">
+      <c r="A80" s="23"/>
+      <c r="B80" s="24"/>
+      <c r="C80" s="25"/>
+      <c r="D80" s="25"/>
+      <c r="E80" s="25"/>
+      <c r="F80" s="25"/>
+      <c r="G80" s="70"/>
+      <c r="H80" s="70"/>
+      <c r="I80" s="25"/>
+      <c r="J80" s="26"/>
+      <c r="K80" s="26"/>
+      <c r="L80" s="27"/>
+      <c r="M80" s="15"/>
+    </row>
+    <row r="82" spans="1:13">
+      <c r="A82" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="B81" s="31"/>
-      <c r="C81" s="31"/>
-      <c r="D81" s="31"/>
-      <c r="E81" s="81"/>
-      <c r="F81" s="44" t="s">
+      <c r="B82" s="31"/>
+      <c r="C82" s="31"/>
+      <c r="D82" s="31"/>
+      <c r="E82" s="81"/>
+      <c r="F82" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="G81" s="44"/>
-      <c r="H81" s="44"/>
-      <c r="I81" s="44"/>
-      <c r="J81" s="43"/>
-      <c r="K81" s="43"/>
-      <c r="L81" s="43"/>
-      <c r="M81" s="43"/>
-    </row>
-    <row r="82" spans="1:13">
-      <c r="A82" s="47" t="s">
+      <c r="G82" s="44"/>
+      <c r="H82" s="44"/>
+      <c r="I82" s="44"/>
+      <c r="J82" s="43"/>
+      <c r="K82" s="43"/>
+      <c r="L82" s="43"/>
+      <c r="M82" s="43"/>
+    </row>
+    <row r="83" spans="1:13">
+      <c r="A83" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B82" s="42" t="s">
+      <c r="B83" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="C82" s="42"/>
-      <c r="D82" s="42"/>
-      <c r="E82" s="82"/>
-      <c r="F82" s="67"/>
-      <c r="G82" s="67"/>
-      <c r="H82" s="67"/>
-      <c r="I82" s="67"/>
-      <c r="J82" s="44"/>
-      <c r="K82" s="45"/>
-      <c r="L82" s="45"/>
-      <c r="M82" s="35"/>
-    </row>
-    <row r="83" spans="1:13">
-      <c r="A83" s="51"/>
-      <c r="B83" s="46"/>
-      <c r="C83" s="38"/>
-      <c r="D83" s="38"/>
-      <c r="E83" s="39"/>
-      <c r="F83" s="68"/>
-      <c r="G83" s="68"/>
-      <c r="H83" s="68"/>
-      <c r="I83" s="34"/>
-      <c r="J83" s="36"/>
-      <c r="K83" s="36"/>
-      <c r="L83" s="36"/>
+      <c r="C83" s="42"/>
+      <c r="D83" s="42"/>
+      <c r="E83" s="82"/>
+      <c r="F83" s="67"/>
+      <c r="G83" s="67"/>
+      <c r="H83" s="67"/>
+      <c r="I83" s="67"/>
+      <c r="J83" s="44"/>
+      <c r="K83" s="45"/>
+      <c r="L83" s="45"/>
       <c r="M83" s="35"/>
     </row>
     <row r="84" spans="1:13">
       <c r="A84" s="51"/>
       <c r="B84" s="46"/>
-      <c r="C84" s="40"/>
-      <c r="D84" s="40"/>
-      <c r="E84" s="41"/>
+      <c r="C84" s="38"/>
+      <c r="D84" s="38"/>
+      <c r="E84" s="39"/>
       <c r="F84" s="68"/>
       <c r="G84" s="68"/>
       <c r="H84" s="68"/>
@@ -3613,11 +3665,11 @@
       <c r="M84" s="35"/>
     </row>
     <row r="85" spans="1:13">
-      <c r="A85" s="52"/>
-      <c r="B85" s="48"/>
-      <c r="C85" s="49"/>
-      <c r="D85" s="49"/>
-      <c r="E85" s="50"/>
+      <c r="A85" s="51"/>
+      <c r="B85" s="46"/>
+      <c r="C85" s="40"/>
+      <c r="D85" s="40"/>
+      <c r="E85" s="41"/>
       <c r="F85" s="68"/>
       <c r="G85" s="68"/>
       <c r="H85" s="68"/>
@@ -3628,22 +3680,23 @@
       <c r="M85" s="35"/>
     </row>
     <row r="86" spans="1:13">
-      <c r="A86" s="13"/>
-      <c r="B86" s="13"/>
-      <c r="C86" s="13"/>
-      <c r="D86" s="13"/>
-      <c r="E86" s="13"/>
-      <c r="F86" s="13"/>
-      <c r="G86" s="13"/>
-      <c r="H86" s="13"/>
-      <c r="I86" s="13"/>
-      <c r="J86" s="13"/>
+      <c r="A86" s="52"/>
+      <c r="B86" s="48"/>
+      <c r="C86" s="49"/>
+      <c r="D86" s="49"/>
+      <c r="E86" s="50"/>
+      <c r="F86" s="68"/>
+      <c r="G86" s="68"/>
+      <c r="H86" s="68"/>
+      <c r="I86" s="34"/>
+      <c r="J86" s="36"/>
+      <c r="K86" s="36"/>
+      <c r="L86" s="36"/>
+      <c r="M86" s="35"/>
     </row>
     <row r="87" spans="1:13">
       <c r="A87" s="13"/>
-      <c r="B87" s="13" t="s">
-        <v>69</v>
-      </c>
+      <c r="B87" s="13"/>
       <c r="C87" s="13"/>
       <c r="D87" s="13"/>
       <c r="E87" s="13"/>
@@ -3654,83 +3707,79 @@
       <c r="J87" s="13"/>
     </row>
     <row r="88" spans="1:13">
-      <c r="A88" s="3" t="s">
+      <c r="A88" s="13"/>
+      <c r="B88" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C88" s="13"/>
+      <c r="D88" s="13"/>
+      <c r="E88" s="13"/>
+      <c r="F88" s="13"/>
+      <c r="G88" s="13"/>
+      <c r="H88" s="13"/>
+      <c r="I88" s="13"/>
+      <c r="J88" s="13"/>
+    </row>
+    <row r="89" spans="1:13">
+      <c r="A89" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B88" s="14"/>
-      <c r="C88" s="14"/>
-      <c r="D88" s="14"/>
-      <c r="E88" s="14"/>
-      <c r="F88" s="14"/>
-      <c r="G88" s="14"/>
-      <c r="H88" s="14"/>
-      <c r="I88" s="14"/>
-      <c r="J88" s="14"/>
-      <c r="K88" s="14"/>
-      <c r="L88" s="6"/>
-      <c r="M88" s="15"/>
-    </row>
-    <row r="89" spans="1:13" ht="13.5" customHeight="1">
-      <c r="A89" s="98" t="s">
+      <c r="B89" s="14"/>
+      <c r="C89" s="14"/>
+      <c r="D89" s="14"/>
+      <c r="E89" s="14"/>
+      <c r="F89" s="14"/>
+      <c r="G89" s="14"/>
+      <c r="H89" s="14"/>
+      <c r="I89" s="14"/>
+      <c r="J89" s="14"/>
+      <c r="K89" s="14"/>
+      <c r="L89" s="6"/>
+      <c r="M89" s="15"/>
+    </row>
+    <row r="90" spans="1:13" ht="13.5" customHeight="1">
+      <c r="A90" s="101" t="s">
         <v>7</v>
       </c>
-      <c r="B89" s="98" t="s">
+      <c r="B90" s="101" t="s">
         <v>68</v>
       </c>
-      <c r="C89" s="97" t="s">
+      <c r="C90" s="98" t="s">
         <v>70</v>
       </c>
-      <c r="D89" s="97" t="s">
+      <c r="D90" s="98" t="s">
         <v>71</v>
       </c>
-      <c r="E89" s="97" t="s">
+      <c r="E90" s="98" t="s">
         <v>65</v>
       </c>
-      <c r="F89" s="108"/>
-      <c r="G89" s="108"/>
-      <c r="H89" s="108"/>
-      <c r="I89" s="110"/>
-      <c r="J89" s="97"/>
-      <c r="K89" s="16"/>
-      <c r="L89" s="17"/>
-      <c r="M89" s="9"/>
-    </row>
-    <row r="90" spans="1:13">
-      <c r="A90" s="98"/>
-      <c r="B90" s="98"/>
-      <c r="C90" s="97"/>
-      <c r="D90" s="97"/>
-      <c r="E90" s="97"/>
-      <c r="F90" s="109"/>
-      <c r="G90" s="109"/>
-      <c r="H90" s="109"/>
-      <c r="I90" s="110"/>
-      <c r="J90" s="97"/>
-      <c r="K90" s="18"/>
-      <c r="L90" s="29"/>
-      <c r="M90" s="15"/>
+      <c r="F90" s="95"/>
+      <c r="G90" s="95"/>
+      <c r="H90" s="95"/>
+      <c r="I90" s="97"/>
+      <c r="J90" s="98"/>
+      <c r="K90" s="16"/>
+      <c r="L90" s="17"/>
+      <c r="M90" s="9"/>
     </row>
     <row r="91" spans="1:13">
-      <c r="A91" s="19">
-        <v>1</v>
-      </c>
-      <c r="B91" s="71"/>
-      <c r="C91" s="78"/>
-      <c r="D91" s="20"/>
-      <c r="E91" s="20"/>
-      <c r="F91" s="90"/>
-      <c r="G91" s="92"/>
-      <c r="H91" s="92"/>
-      <c r="I91" s="90"/>
-      <c r="J91" s="21"/>
-      <c r="K91" s="21"/>
-      <c r="L91" s="28"/>
+      <c r="A91" s="101"/>
+      <c r="B91" s="101"/>
+      <c r="C91" s="98"/>
+      <c r="D91" s="98"/>
+      <c r="E91" s="98"/>
+      <c r="F91" s="96"/>
+      <c r="G91" s="96"/>
+      <c r="H91" s="96"/>
+      <c r="I91" s="97"/>
+      <c r="J91" s="98"/>
+      <c r="K91" s="18"/>
+      <c r="L91" s="29"/>
       <c r="M91" s="15"/>
     </row>
     <row r="92" spans="1:13">
       <c r="A92" s="19">
-        <f>A91+1</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B92" s="71"/>
       <c r="C92" s="78"/>
@@ -3747,11 +3796,11 @@
     </row>
     <row r="93" spans="1:13">
       <c r="A93" s="19">
-        <f t="shared" ref="A93:A97" si="1">A92+1</f>
-        <v>3</v>
-      </c>
-      <c r="B93" s="72"/>
-      <c r="C93" s="79"/>
+        <f>A92+1</f>
+        <v>2</v>
+      </c>
+      <c r="B93" s="71"/>
+      <c r="C93" s="78"/>
       <c r="D93" s="20"/>
       <c r="E93" s="20"/>
       <c r="F93" s="90"/>
@@ -3760,16 +3809,16 @@
       <c r="I93" s="90"/>
       <c r="J93" s="21"/>
       <c r="K93" s="21"/>
-      <c r="L93" s="22"/>
+      <c r="L93" s="28"/>
       <c r="M93" s="15"/>
     </row>
     <row r="94" spans="1:13">
       <c r="A94" s="19">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="B94" s="73"/>
-      <c r="C94" s="80"/>
+        <f t="shared" ref="A94:A98" si="1">A93+1</f>
+        <v>3</v>
+      </c>
+      <c r="B94" s="72"/>
+      <c r="C94" s="79"/>
       <c r="D94" s="20"/>
       <c r="E94" s="20"/>
       <c r="F94" s="90"/>
@@ -3784,7 +3833,7 @@
     <row r="95" spans="1:13">
       <c r="A95" s="19">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B95" s="73"/>
       <c r="C95" s="80"/>
@@ -3802,84 +3851,103 @@
     <row r="96" spans="1:13">
       <c r="A96" s="19">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B96" s="73"/>
       <c r="C96" s="80"/>
-      <c r="D96" s="74"/>
-      <c r="E96" s="74"/>
-      <c r="F96" s="91"/>
-      <c r="G96" s="93"/>
-      <c r="H96" s="93"/>
-      <c r="I96" s="91"/>
-      <c r="J96" s="76"/>
-      <c r="K96" s="76"/>
-      <c r="L96" s="77"/>
+      <c r="D96" s="20"/>
+      <c r="E96" s="20"/>
+      <c r="F96" s="90"/>
+      <c r="G96" s="92"/>
+      <c r="H96" s="92"/>
+      <c r="I96" s="90"/>
+      <c r="J96" s="21"/>
+      <c r="K96" s="21"/>
+      <c r="L96" s="22"/>
       <c r="M96" s="15"/>
     </row>
     <row r="97" spans="1:13">
       <c r="A97" s="19">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B97" s="73"/>
       <c r="C97" s="80"/>
-      <c r="D97" s="20"/>
-      <c r="E97" s="20"/>
-      <c r="F97" s="90"/>
-      <c r="G97" s="92"/>
-      <c r="H97" s="92"/>
-      <c r="I97" s="90"/>
-      <c r="J97" s="21"/>
-      <c r="K97" s="21"/>
-      <c r="L97" s="22"/>
+      <c r="D97" s="74"/>
+      <c r="E97" s="74"/>
+      <c r="F97" s="91"/>
+      <c r="G97" s="93"/>
+      <c r="H97" s="93"/>
+      <c r="I97" s="91"/>
+      <c r="J97" s="76"/>
+      <c r="K97" s="76"/>
+      <c r="L97" s="77"/>
       <c r="M97" s="15"/>
     </row>
+    <row r="98" spans="1:13">
+      <c r="A98" s="19">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="B98" s="73"/>
+      <c r="C98" s="80"/>
+      <c r="D98" s="20"/>
+      <c r="E98" s="20"/>
+      <c r="F98" s="90"/>
+      <c r="G98" s="92"/>
+      <c r="H98" s="92"/>
+      <c r="I98" s="90"/>
+      <c r="J98" s="21"/>
+      <c r="K98" s="21"/>
+      <c r="L98" s="22"/>
+      <c r="M98" s="15"/>
+    </row>
   </sheetData>
-  <mergeCells count="26">
-    <mergeCell ref="F89:F90"/>
-    <mergeCell ref="H89:H90"/>
-    <mergeCell ref="I89:J90"/>
-    <mergeCell ref="G60:G61"/>
-    <mergeCell ref="G89:G90"/>
-    <mergeCell ref="A89:A90"/>
-    <mergeCell ref="B89:B90"/>
-    <mergeCell ref="C89:C90"/>
-    <mergeCell ref="D89:D90"/>
-    <mergeCell ref="E89:E90"/>
+  <mergeCells count="27">
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="I61:J62"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="C61:C62"/>
+    <mergeCell ref="E61:E62"/>
+    <mergeCell ref="D61:D62"/>
+    <mergeCell ref="H61:H62"/>
+    <mergeCell ref="F61:F62"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A24:B24"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="C14:E14"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="I60:J61"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="E60:E61"/>
-    <mergeCell ref="D60:D61"/>
-    <mergeCell ref="H60:H61"/>
-    <mergeCell ref="F60:F61"/>
-    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A90:A91"/>
+    <mergeCell ref="B90:B91"/>
+    <mergeCell ref="C90:C91"/>
+    <mergeCell ref="D90:D91"/>
+    <mergeCell ref="E90:E91"/>
+    <mergeCell ref="F90:F91"/>
+    <mergeCell ref="H90:H91"/>
+    <mergeCell ref="I90:J91"/>
+    <mergeCell ref="G61:G62"/>
+    <mergeCell ref="G90:G91"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E101:H101" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E102:H102" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C25:C26" xr:uid="{78FE03A8-B82F-DD42-A5B2-F5AED31EB8E5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C26:C27" xr:uid="{78FE03A8-B82F-DD42-A5B2-F5AED31EB8E5}">
       <formula1>adjustFiledName</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C16" xr:uid="{0933AF92-3C0C-2F47-AF58-F84946F39270}">
       <formula1>componentKind</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F62:G79 C17:C23" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F63:G80 C17:C23" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
       <formula1>yesNo</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C24" xr:uid="{CCFC1331-CEEF-574E-9BCC-37D38F486896}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C25" xr:uid="{CCFC1331-CEEF-574E-9BCC-37D38F486896}">
       <formula1>adjustFieldName</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>